<commit_message>
Modified the structure to add the new fields
</commit_message>
<xml_diff>
--- a/Weather/bin/newFile.xlsx
+++ b/Weather/bin/newFile.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
   <si>
     <t>Time Stamp</t>
   </si>
@@ -87,6 +87,33 @@
   </si>
   <si>
     <t>2017.05.21 15.51.35</t>
+  </si>
+  <si>
+    <t>2017.05.29 03.41.21</t>
+  </si>
+  <si>
+    <t>2017-05-29T09:00:00</t>
+  </si>
+  <si>
+    <t>2017-05-29T12:00:00</t>
+  </si>
+  <si>
+    <t>2017.05.29 03.41.47</t>
+  </si>
+  <si>
+    <t>2017.05.29 03.42.21</t>
+  </si>
+  <si>
+    <t>2017.05.29 03.42.39</t>
+  </si>
+  <si>
+    <t>2017.05.29 03.43.42</t>
+  </si>
+  <si>
+    <t>2017.05.29 03.52.32</t>
+  </si>
+  <si>
+    <t>2017.05.29 03.58.20</t>
   </si>
 </sst>
 </file>
@@ -402,7 +429,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -644,6 +671,281 @@
         <v>2.359999895095825</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="n">
+        <v>15.539999961853027</v>
+      </c>
+      <c r="C7" t="n">
+        <v>87.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1014.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="n">
+        <v>14.079999923706055</v>
+      </c>
+      <c r="I7" t="n">
+        <v>995.1799926757812</v>
+      </c>
+      <c r="J7" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.3100000023841858</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="n">
+        <v>15.539999961853027</v>
+      </c>
+      <c r="C8" t="n">
+        <v>87.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1014.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="n">
+        <v>14.079999923706055</v>
+      </c>
+      <c r="I8" t="n">
+        <v>995.1799926757812</v>
+      </c>
+      <c r="J8" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.3100000023841858</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="n">
+        <v>15.539999961853027</v>
+      </c>
+      <c r="C9" t="n">
+        <v>87.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1014.0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="n">
+        <v>14.079999923706055</v>
+      </c>
+      <c r="I9" t="n">
+        <v>995.1799926757812</v>
+      </c>
+      <c r="J9" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.3100000023841858</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="n">
+        <v>15.539999961853027</v>
+      </c>
+      <c r="C10" t="n">
+        <v>87.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1014.0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" t="n">
+        <v>14.079999923706055</v>
+      </c>
+      <c r="I10" t="n">
+        <v>995.1799926757812</v>
+      </c>
+      <c r="J10" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.3100000023841858</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="n">
+        <v>15.539999961853027</v>
+      </c>
+      <c r="C11" t="n">
+        <v>87.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1014.0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="n">
+        <v>14.079999923706055</v>
+      </c>
+      <c r="I11" t="n">
+        <v>995.1799926757812</v>
+      </c>
+      <c r="J11" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.3100000023841858</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="n">
+        <v>15.539999961853027</v>
+      </c>
+      <c r="C12" t="n">
+        <v>87.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1014.0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" t="n">
+        <v>14.079999923706055</v>
+      </c>
+      <c r="I12" t="n">
+        <v>995.1799926757812</v>
+      </c>
+      <c r="J12" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.3100000023841858</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="n">
+        <v>15.539999961853027</v>
+      </c>
+      <c r="C13" t="n">
+        <v>87.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1014.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" t="n">
+        <v>14.079999923706055</v>
+      </c>
+      <c r="I13" t="n">
+        <v>995.1799926757812</v>
+      </c>
+      <c r="J13" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" t="s">
+        <v>15</v>
+      </c>
+      <c r="M13" t="s">
+        <v>15</v>
+      </c>
+      <c r="N13" t="s">
+        <v>15</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.3100000023841858</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
ML code is added
</commit_message>
<xml_diff>
--- a/Weather/bin/newFile.xlsx
+++ b/Weather/bin/newFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>Time Stamp</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>2017.05.30 02.41.39</t>
+  </si>
+  <si>
+    <t>2017.05.30 02.59.50</t>
+  </si>
+  <si>
+    <t>2017.05.30 03.00.27</t>
+  </si>
+  <si>
+    <t>2017.05.30 03.00.48</t>
   </si>
 </sst>
 </file>
@@ -396,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G18" sqref="A1:P146"/>
@@ -820,6 +829,138 @@
         <v>83.90000000000001</v>
       </c>
     </row>
+    <row r="19" spans="1:15">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="n">
+        <v>15.14999961853027</v>
+      </c>
+      <c r="C19" t="n">
+        <v>100</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1013</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" t="n">
+        <v>15.07999992370605</v>
+      </c>
+      <c r="I19" t="n">
+        <v>994.3699951171875</v>
+      </c>
+      <c r="J19" t="n">
+        <v>100</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.05999999865889549</v>
+      </c>
+      <c r="L19" t="n">
+        <v>1.610000014305115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="n">
+        <v>15.14999961853027</v>
+      </c>
+      <c r="C20" t="n">
+        <v>100</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1013</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" t="n">
+        <v>15.07999992370605</v>
+      </c>
+      <c r="I20" t="n">
+        <v>994.3699951171875</v>
+      </c>
+      <c r="J20" t="n">
+        <v>100</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.05999999865889549</v>
+      </c>
+      <c r="L20" t="n">
+        <v>1.610000014305115</v>
+      </c>
+      <c r="M20" t="n">
+        <v>16.98</v>
+      </c>
+      <c r="N20" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="O20" t="n">
+        <v>84.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="n">
+        <v>15.14999961853027</v>
+      </c>
+      <c r="C21" t="n">
+        <v>100</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1013</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" t="n">
+        <v>15.07999992370605</v>
+      </c>
+      <c r="I21" t="n">
+        <v>994.3699951171875</v>
+      </c>
+      <c r="J21" t="n">
+        <v>100</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.05999999865889549</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1.610000014305115</v>
+      </c>
+      <c r="M21" t="n">
+        <v>17</v>
+      </c>
+      <c r="N21" t="n">
+        <v>2.34</v>
+      </c>
+      <c r="O21" t="n">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
the predicted value is being sent serially through python
</commit_message>
<xml_diff>
--- a/Weather/bin/newFile.xlsx
+++ b/Weather/bin/newFile.xlsx
@@ -1,33 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/balaji/Documents/Github/IOT/Weather/src/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="15460" windowWidth="25600" xWindow="0" yWindow="460"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Current Weather" r:id="rId1" sheetId="1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Current Weather" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>Time Stamp</t>
   </si>
@@ -86,9 +73,6 @@
     <t>2017-06-02T06:00:00</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>2017.06.01 20.23.17</t>
   </si>
   <si>
@@ -105,43 +89,55 @@
   </si>
   <si>
     <t>2017.06.01 20.23.26</t>
+  </si>
+  <si>
+    <t>2017.06.01 20.44.35</t>
+  </si>
+  <si>
+    <t>2017.06.01 20.44.37</t>
+  </si>
+  <si>
+    <t>2017.06.01 20.44.38</t>
+  </si>
+  <si>
+    <t>2017.06.01 20.44.39</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000;[Red]0.0000"/>
+    <numFmt formatCode="0.0000;[Red]0.0000" numFmtId="164"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="12"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="11"/>
+      <sz val="12"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -162,21 +158,15 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="1"/>
     <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="2"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -185,10 +175,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -223,7 +213,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -258,7 +248,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -352,21 +342,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -383,7 +373,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -435,42 +425,46 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView showRuler="0" tabSelected="1" topLeftCell="F97" workbookViewId="0">
-      <selection activeCell="O114" sqref="A1:XFD1048576"/>
+    <sheetView showRuler="0" tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="17.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="18.83203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="11.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.83203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="16.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="21.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="19.1640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="22.83203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="20.5" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="20.83203125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="25.33203125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="15.1640625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="24.33203125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="15.1640625" collapsed="true"/>
-    <col min="16" max="20" customWidth="true" style="1" width="10.83203125" collapsed="true"/>
-    <col min="21" max="16384" style="1" width="10.83203125" collapsed="true"/>
+    <col bestFit="1" collapsed="1" customWidth="1" max="1" min="1" style="1" width="17.6640625"/>
+    <col bestFit="1" collapsed="1" customWidth="1" max="2" min="2" style="1" width="18.83203125"/>
+    <col bestFit="1" collapsed="1" customWidth="1" max="3" min="3" style="1" width="11.6640625"/>
+    <col bestFit="1" collapsed="1" customWidth="1" max="4" min="4" style="1" width="12.83203125"/>
+    <col bestFit="1" collapsed="1" customWidth="1" max="5" min="5" style="1" width="16"/>
+    <col bestFit="1" collapsed="1" customWidth="1" max="6" min="6" style="1" width="21.33203125"/>
+    <col bestFit="1" collapsed="1" customWidth="1" max="7" min="7" style="1" width="19.1640625"/>
+    <col bestFit="1" collapsed="1" customWidth="1" max="8" min="8" style="1" width="28.33203125"/>
+    <col bestFit="1" collapsed="1" customWidth="1" max="9" min="9" style="1" width="22.83203125"/>
+    <col bestFit="1" collapsed="1" customWidth="1" max="10" min="10" style="1" width="20.5"/>
+    <col bestFit="1" collapsed="1" customWidth="1" max="11" min="11" style="1" width="20.83203125"/>
+    <col bestFit="1" collapsed="1" customWidth="1" max="12" min="12" style="1" width="25.33203125"/>
+    <col bestFit="1" collapsed="1" customWidth="1" max="13" min="13" style="1" width="15.1640625"/>
+    <col bestFit="1" collapsed="1" customWidth="1" max="14" min="14" style="1" width="24.33203125"/>
+    <col bestFit="1" collapsed="1" customWidth="1" max="15" min="15" style="1" width="15.1640625"/>
+    <col collapsed="1" customWidth="1" max="20" min="16" style="1" width="10.83203125"/>
+    <col collapsed="1" customWidth="1" max="16384" min="21" style="1" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,21 +514,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="n">
-        <v>19.229999542236328</v>
+        <v>19.22999954223633</v>
       </c>
       <c r="C2" t="n">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="D2" t="n">
-        <v>1011.0</v>
+        <v>1011</v>
       </c>
       <c r="E2" t="n">
-        <v>2.5999999046325684</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -549,39 +543,42 @@
         <v>994.260009765625</v>
       </c>
       <c r="J2" t="n">
-        <v>97.0</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
+        <v>97</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
       </c>
       <c r="L2" t="n">
         <v>1.159999966621399</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>800</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="N2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
       <c r="B3" t="n">
-        <v>19.229999542236328</v>
+        <v>19.22999954223633</v>
       </c>
       <c r="C3" t="n">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="D3" t="n">
-        <v>1011.0</v>
+        <v>1011</v>
       </c>
       <c r="E3" t="n">
-        <v>2.5999999046325684</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -596,39 +593,42 @@
         <v>994.260009765625</v>
       </c>
       <c r="J3" t="n">
-        <v>97.0</v>
-      </c>
-      <c r="K3" t="s">
-        <v>19</v>
+        <v>97</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
       </c>
       <c r="L3" t="n">
         <v>1.159999966621399</v>
       </c>
-      <c r="M3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>890</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" t="n">
-        <v>19.229999542236328</v>
+        <v>19.22999954223633</v>
       </c>
       <c r="C4" t="n">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="D4" t="n">
-        <v>1011.0</v>
+        <v>1011</v>
       </c>
       <c r="E4" t="n">
-        <v>2.5999999046325684</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -643,39 +643,42 @@
         <v>994.260009765625</v>
       </c>
       <c r="J4" t="n">
-        <v>97.0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>19</v>
+        <v>97</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
       </c>
       <c r="L4" t="n">
         <v>1.159999966621399</v>
       </c>
-      <c r="M4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>800</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="n">
-        <v>19.229999542236328</v>
+        <v>19.22999954223633</v>
       </c>
       <c r="C5" t="n">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="D5" t="n">
-        <v>1011.0</v>
+        <v>1011</v>
       </c>
       <c r="E5" t="n">
-        <v>2.5999999046325684</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -690,39 +693,42 @@
         <v>994.260009765625</v>
       </c>
       <c r="J5" t="n">
-        <v>97.0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>19</v>
+        <v>97</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
       </c>
       <c r="L5" t="n">
         <v>1.159999966621399</v>
       </c>
-      <c r="M5" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>890</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" t="n">
-        <v>19.229999542236328</v>
+        <v>19.22999954223633</v>
       </c>
       <c r="C6" t="n">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="D6" t="n">
-        <v>1011.0</v>
+        <v>1011</v>
       </c>
       <c r="E6" t="n">
-        <v>2.5999999046325684</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -737,39 +743,42 @@
         <v>994.260009765625</v>
       </c>
       <c r="J6" t="n">
-        <v>97.0</v>
-      </c>
-      <c r="K6" t="s">
-        <v>19</v>
+        <v>97</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
       </c>
       <c r="L6" t="n">
         <v>1.159999966621399</v>
       </c>
-      <c r="M6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>800</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="n">
-        <v>19.229999542236328</v>
+        <v>19.22999954223633</v>
       </c>
       <c r="C7" t="n">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="D7" t="n">
-        <v>1011.0</v>
+        <v>1011</v>
       </c>
       <c r="E7" t="n">
-        <v>2.5999999046325684</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -784,39 +793,42 @@
         <v>994.260009765625</v>
       </c>
       <c r="J7" t="n">
-        <v>97.0</v>
-      </c>
-      <c r="K7" t="s">
-        <v>19</v>
+        <v>97</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
       </c>
       <c r="L7" t="n">
         <v>1.159999966621399</v>
       </c>
-      <c r="M7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>890</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="n">
-        <v>19.229999542236328</v>
+        <v>19.22999954223633</v>
       </c>
       <c r="C8" t="n">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="D8" t="n">
-        <v>1011.0</v>
+        <v>1011</v>
       </c>
       <c r="E8" t="n">
-        <v>2.5999999046325684</v>
+        <v>2.599999904632568</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
@@ -831,22 +843,225 @@
         <v>994.260009765625</v>
       </c>
       <c r="J8" t="n">
-        <v>97.0</v>
-      </c>
-      <c r="K8" t="s">
-        <v>19</v>
+        <v>97</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
       </c>
       <c r="L8" t="n">
         <v>1.159999966621399</v>
       </c>
-      <c r="M8" t="s">
-        <v>19</v>
-      </c>
-      <c r="N8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O8" t="s">
-        <v>19</v>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>800</v>
+      </c>
+      <c r="P8" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="n">
+        <v>19.22999954223633</v>
+      </c>
+      <c r="C9" t="n">
+        <v>72</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1011</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2.599999904632568</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="n">
+        <v>12.6899995803833</v>
+      </c>
+      <c r="I9" t="n">
+        <v>994.260009765625</v>
+      </c>
+      <c r="J9" t="n">
+        <v>97</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1.159999966621399</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>890</v>
+      </c>
+      <c r="P9" t="n">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="n">
+        <v>19.22999954223633</v>
+      </c>
+      <c r="C10" t="n">
+        <v>72</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1011</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2.599999904632568</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="n">
+        <v>12.6899995803833</v>
+      </c>
+      <c r="I10" t="n">
+        <v>994.260009765625</v>
+      </c>
+      <c r="J10" t="n">
+        <v>97</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1.159999966621399</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>800</v>
+      </c>
+      <c r="P10" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="n">
+        <v>19.22999954223633</v>
+      </c>
+      <c r="C11" t="n">
+        <v>72</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1011</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2.599999904632568</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" t="n">
+        <v>12.6899995803833</v>
+      </c>
+      <c r="I11" t="n">
+        <v>994.260009765625</v>
+      </c>
+      <c r="J11" t="n">
+        <v>97</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1.159999966621399</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>890</v>
+      </c>
+      <c r="P11" t="n">
+        <v>847.4545454545456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="n">
+        <v>19.22999954223633</v>
+      </c>
+      <c r="C12" t="n">
+        <v>72</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1011</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2.599999904632568</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" t="n">
+        <v>12.6899995803833</v>
+      </c>
+      <c r="I12" t="n">
+        <v>994.260009765625</v>
+      </c>
+      <c r="J12" t="n">
+        <v>97</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1.159999966621399</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>800</v>
+      </c>
+      <c r="P12" t="n">
+        <v>839.2727272727274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Code but the threads have to work
</commit_message>
<xml_diff>
--- a/Weather/bin/newFile.xlsx
+++ b/Weather/bin/newFile.xlsx
@@ -6,15 +6,14 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Current Weather" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Current Weather" r:id="rId1" sheetId="1" state="visible"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55" count="6">
   <si>
     <t>Time Stamp</t>
   </si>
@@ -101,6 +100,84 @@
   </si>
   <si>
     <t>2017.06.01 20.44.39</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.00.37</t>
+  </si>
+  <si>
+    <t>2017-06-04T00:00:00</t>
+  </si>
+  <si>
+    <t>2017-06-04T03:00:00</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.00.39</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.00.40</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.00.42</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.00.43</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.00.44</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.00.46</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.00.47</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.00.48</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.00.49</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.00.51</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.03.31</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.03.52</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.04.13</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.04.33</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.25.28</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.26.48</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.27.49</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.28.50</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.32.42</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.33.43</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.34.44</t>
+  </si>
+  <si>
+    <t>2017.06.03 19.35.44</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -108,7 +185,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="0.0000;[Red]0.0000" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="0.0000;[Red]0.0000"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -175,10 +252,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -213,7 +290,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -248,7 +325,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -342,21 +419,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -373,7 +450,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -425,7 +502,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -437,31 +514,31 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView showRuler="0" tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView showRuler="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
   <cols>
-    <col bestFit="1" collapsed="1" customWidth="1" max="1" min="1" style="1" width="17.6640625"/>
-    <col bestFit="1" collapsed="1" customWidth="1" max="2" min="2" style="1" width="18.83203125"/>
-    <col bestFit="1" collapsed="1" customWidth="1" max="3" min="3" style="1" width="11.6640625"/>
-    <col bestFit="1" collapsed="1" customWidth="1" max="4" min="4" style="1" width="12.83203125"/>
-    <col bestFit="1" collapsed="1" customWidth="1" max="5" min="5" style="1" width="16"/>
-    <col bestFit="1" collapsed="1" customWidth="1" max="6" min="6" style="1" width="21.33203125"/>
-    <col bestFit="1" collapsed="1" customWidth="1" max="7" min="7" style="1" width="19.1640625"/>
-    <col bestFit="1" collapsed="1" customWidth="1" max="8" min="8" style="1" width="28.33203125"/>
-    <col bestFit="1" collapsed="1" customWidth="1" max="9" min="9" style="1" width="22.83203125"/>
-    <col bestFit="1" collapsed="1" customWidth="1" max="10" min="10" style="1" width="20.5"/>
-    <col bestFit="1" collapsed="1" customWidth="1" max="11" min="11" style="1" width="20.83203125"/>
-    <col bestFit="1" collapsed="1" customWidth="1" max="12" min="12" style="1" width="25.33203125"/>
-    <col bestFit="1" collapsed="1" customWidth="1" max="13" min="13" style="1" width="15.1640625"/>
-    <col bestFit="1" collapsed="1" customWidth="1" max="14" min="14" style="1" width="24.33203125"/>
-    <col bestFit="1" collapsed="1" customWidth="1" max="15" min="15" style="1" width="15.1640625"/>
-    <col collapsed="1" customWidth="1" max="20" min="16" style="1" width="10.83203125"/>
-    <col collapsed="1" customWidth="1" max="16384" min="21" style="1" width="10.83203125"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="17.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="18.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="11.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.83203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="16.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="21.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="19.1640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="28.33203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="22.83203125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="20.5" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="20.83203125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="25.33203125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="15.1640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="24.33203125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="15.1640625" collapsed="true"/>
+    <col min="16" max="22" customWidth="true" style="1" width="10.83203125" collapsed="true"/>
+    <col min="23" max="16384" customWidth="true" style="1" width="10.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -1052,16 +1129,1157 @@
         <v>1.159999966621399</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>46.32</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>2.45</v>
       </c>
       <c r="O12" t="n">
+        <v>40.1</v>
+      </c>
+      <c r="P12" t="n">
+        <v>789.279090909091</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="n">
+        <v>22.6200008392334</v>
+      </c>
+      <c r="C13" t="n">
+        <v>82</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5.699999809265137</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" t="n">
+        <v>18.59000015258789</v>
+      </c>
+      <c r="I13" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J13" t="n">
+        <v>76</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
         <v>800</v>
       </c>
-      <c r="P12" t="n">
-        <v>839.2727272727274</v>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="n">
+        <v>22.6200008392334</v>
+      </c>
+      <c r="C14" t="n">
+        <v>82</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E14" t="n">
+        <v>5.699999809265137</v>
+      </c>
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" t="n">
+        <v>18.59000015258789</v>
+      </c>
+      <c r="I14" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J14" t="n">
+        <v>76</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>829</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="n">
+        <v>22.6200008392334</v>
+      </c>
+      <c r="C15" t="n">
+        <v>82</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E15" t="n">
+        <v>5.699999809265137</v>
+      </c>
+      <c r="F15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" t="n">
+        <v>18.59000015258789</v>
+      </c>
+      <c r="I15" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J15" t="n">
+        <v>76</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>810</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="n">
+        <v>22.6200008392334</v>
+      </c>
+      <c r="C16" t="n">
+        <v>82</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E16" t="n">
+        <v>5.699999809265137</v>
+      </c>
+      <c r="F16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" t="n">
+        <v>18.59000015258789</v>
+      </c>
+      <c r="I16" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J16" t="n">
+        <v>76</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>800</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="n">
+        <v>22.6200008392334</v>
+      </c>
+      <c r="C17" t="n">
+        <v>82</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E17" t="n">
+        <v>5.699999809265137</v>
+      </c>
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" t="n">
+        <v>18.59000015258789</v>
+      </c>
+      <c r="I17" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J17" t="n">
+        <v>76</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>790</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="n">
+        <v>22.6200008392334</v>
+      </c>
+      <c r="C18" t="n">
+        <v>82</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E18" t="n">
+        <v>5.699999809265137</v>
+      </c>
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" t="n">
+        <v>18.59000015258789</v>
+      </c>
+      <c r="I18" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J18" t="n">
+        <v>76</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>780</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="n">
+        <v>22.6200008392334</v>
+      </c>
+      <c r="C19" t="n">
+        <v>82</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E19" t="n">
+        <v>5.699999809265137</v>
+      </c>
+      <c r="F19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" t="n">
+        <v>18.59000015258789</v>
+      </c>
+      <c r="I19" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J19" t="n">
+        <v>76</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>770</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="n">
+        <v>22.6200008392334</v>
+      </c>
+      <c r="C20" t="n">
+        <v>82</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E20" t="n">
+        <v>5.699999809265137</v>
+      </c>
+      <c r="F20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" t="n">
+        <v>18.59000015258789</v>
+      </c>
+      <c r="I20" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J20" t="n">
+        <v>76</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" t="n">
+        <v>760</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="n">
+        <v>22.6200008392334</v>
+      </c>
+      <c r="C21" t="n">
+        <v>82</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E21" t="n">
+        <v>5.699999809265137</v>
+      </c>
+      <c r="F21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" t="n">
+        <v>18.59000015258789</v>
+      </c>
+      <c r="I21" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J21" t="n">
+        <v>76</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" t="n">
+        <v>750</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="n">
+        <v>22.6200008392334</v>
+      </c>
+      <c r="C22" t="n">
+        <v>82</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E22" t="n">
+        <v>5.699999809265137</v>
+      </c>
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" t="n">
+        <v>18.59000015258789</v>
+      </c>
+      <c r="I22" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J22" t="n">
+        <v>76</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="n">
+        <v>740</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="n">
+        <v>22.6200008392334</v>
+      </c>
+      <c r="C23" t="n">
+        <v>82</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E23" t="n">
+        <v>5.699999809265137</v>
+      </c>
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" t="n">
+        <v>18.59000015258789</v>
+      </c>
+      <c r="I23" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J23" t="n">
+        <v>76</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="n">
+        <v>730</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="n">
+        <v>22.6200008392334</v>
+      </c>
+      <c r="C24" t="n">
+        <v>82</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E24" t="n">
+        <v>5.699999809265137</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" t="n">
+        <v>18.59000015258789</v>
+      </c>
+      <c r="I24" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J24" t="n">
+        <v>76</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="n">
+        <v>720</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" t="n">
+        <v>22.6200008392334</v>
+      </c>
+      <c r="C25" t="n">
+        <v>82</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E25" t="n">
+        <v>5.699999809265137</v>
+      </c>
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" t="n">
+        <v>18.59000015258789</v>
+      </c>
+      <c r="I25" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J25" t="n">
+        <v>76</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M25" t="n">
+        <v>16.31</v>
+      </c>
+      <c r="N25" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="O25" t="n">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="n">
+        <v>22.6200008392334</v>
+      </c>
+      <c r="C26" t="n">
+        <v>82</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E26" t="n">
+        <v>5.699999809265137</v>
+      </c>
+      <c r="F26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26" t="n">
+        <v>18.59000015258789</v>
+      </c>
+      <c r="I26" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J26" t="n">
+        <v>76</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" t="n">
+        <v>700</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" t="n">
+        <v>22.6200008392334</v>
+      </c>
+      <c r="C27" t="n">
+        <v>82</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E27" t="n">
+        <v>5.699999809265137</v>
+      </c>
+      <c r="F27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" t="n">
+        <v>18.59000015258789</v>
+      </c>
+      <c r="I27" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J27" t="n">
+        <v>76</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>690</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="n">
+        <v>21.01000022888184</v>
+      </c>
+      <c r="C28" t="n">
+        <v>82</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E28" t="n">
+        <v>4.599999904632568</v>
+      </c>
+      <c r="F28" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" t="s">
+        <v>31</v>
+      </c>
+      <c r="H28" t="n">
+        <v>17.29999923706055</v>
+      </c>
+      <c r="I28" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J28" t="n">
+        <v>76</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" t="n">
+        <v>680</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="n">
+        <v>21.01000022888184</v>
+      </c>
+      <c r="C29" t="n">
+        <v>82</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E29" t="n">
+        <v>4.599999904632568</v>
+      </c>
+      <c r="F29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" t="s">
+        <v>31</v>
+      </c>
+      <c r="H29" t="n">
+        <v>17.29999923706055</v>
+      </c>
+      <c r="I29" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J29" t="n">
+        <v>76</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M29" t="n">
+        <v>16.52</v>
+      </c>
+      <c r="N29" t="n">
+        <v>2.39</v>
+      </c>
+      <c r="O29" t="n">
+        <v>660</v>
+      </c>
+      <c r="P29" t="n">
+        <v>415.7765141700405</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" t="n">
+        <v>21.01000022888184</v>
+      </c>
+      <c r="C30" t="n">
+        <v>82</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E30" t="n">
+        <v>4.599999904632568</v>
+      </c>
+      <c r="F30" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H30" t="n">
+        <v>17.29999923706055</v>
+      </c>
+      <c r="I30" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J30" t="n">
+        <v>76</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M30" t="n">
+        <v>686.48</v>
+      </c>
+      <c r="N30" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="O30" t="n">
+        <v>640</v>
+      </c>
+      <c r="P30" t="n">
+        <v>265.9794871794873</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" t="n">
+        <v>20.64999961853027</v>
+      </c>
+      <c r="C31" t="n">
+        <v>82</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E31" t="n">
+        <v>4.599999904632568</v>
+      </c>
+      <c r="F31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" t="n">
+        <v>17.29999923706055</v>
+      </c>
+      <c r="I31" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J31" t="n">
+        <v>76</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M31" t="n">
+        <v>686.48</v>
+      </c>
+      <c r="N31" t="n">
+        <v>32</v>
+      </c>
+      <c r="O31" t="n">
+        <v>620</v>
+      </c>
+      <c r="P31" s="1" t="n">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" t="n">
+        <v>20.64999961853027</v>
+      </c>
+      <c r="C32" t="n">
+        <v>82</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E32" t="n">
+        <v>4.599999904632568</v>
+      </c>
+      <c r="F32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" t="n">
+        <v>17.29999923706055</v>
+      </c>
+      <c r="I32" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J32" t="n">
+        <v>76</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M32" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="N32" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="O32" t="n">
+        <v>46.9</v>
+      </c>
+      <c r="P32" t="n">
+        <v>624.2505119047621</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="n">
+        <v>20.64999961853027</v>
+      </c>
+      <c r="C33" t="n">
+        <v>82</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E33" t="n">
+        <v>4.599999904632568</v>
+      </c>
+      <c r="F33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" t="s">
+        <v>31</v>
+      </c>
+      <c r="H33" t="n">
+        <v>17.29999923706055</v>
+      </c>
+      <c r="I33" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J33" t="n">
+        <v>76</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M33" t="n">
+        <v>656.5</v>
+      </c>
+      <c r="N33" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="O33" t="n">
+        <v>46.8</v>
+      </c>
+      <c r="P33" t="n">
+        <v>574.6695773809524</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" t="n">
+        <v>20.64999961853027</v>
+      </c>
+      <c r="C34" t="n">
+        <v>82</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1012</v>
+      </c>
+      <c r="E34" t="n">
+        <v>4.599999904632568</v>
+      </c>
+      <c r="F34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" t="s">
+        <v>31</v>
+      </c>
+      <c r="H34" t="n">
+        <v>17.29999923706055</v>
+      </c>
+      <c r="I34" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J34" t="n">
+        <v>76</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M34" t="n">
+        <v>656.39</v>
+      </c>
+      <c r="N34" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="O34" t="n">
+        <v>46.6</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" t="n">
+        <v>20.649999618530273</v>
+      </c>
+      <c r="C35" t="n">
+        <v>82.0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1012.0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>4.599999904632568</v>
+      </c>
+      <c r="F35" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H35" t="n">
+        <v>17.299999237060547</v>
+      </c>
+      <c r="I35" t="n">
+        <v>993.760009765625</v>
+      </c>
+      <c r="J35" t="n">
+        <v>76.0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L35" t="n">
+        <v>1.2799999713897705</v>
+      </c>
+      <c r="M35" t="s">
+        <v>54</v>
+      </c>
+      <c r="N35" t="s">
+        <v>54</v>
+      </c>
+      <c r="O35" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Modified Code for arduino web server
</commit_message>
<xml_diff>
--- a/Weather/bin/newFile.xlsx
+++ b/Weather/bin/newFile.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55" count="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="59" count="6">
   <si>
     <t>Time Stamp</t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t>2017.06.03 19.35.44</t>
+  </si>
+  <si>
+    <t>2017.06.03 20.14.05</t>
+  </si>
+  <si>
+    <t>2017-06-04T06:00:00</t>
+  </si>
+  <si>
+    <t>2017.06.03 20.15.06</t>
+  </si>
+  <si>
+    <t>2017.06.03 20.16.06</t>
   </si>
   <si>
     <t/>
@@ -514,10 +526,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView showRuler="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView showRuler="0" tabSelected="1" topLeftCell="H16" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
@@ -537,8 +549,8 @@
     <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="15.1640625" collapsed="true"/>
     <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="24.33203125" collapsed="true"/>
     <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="15.1640625" collapsed="true"/>
-    <col min="16" max="22" customWidth="true" style="1" width="10.83203125" collapsed="true"/>
-    <col min="23" max="16384" customWidth="true" style="1" width="10.83203125" collapsed="true"/>
+    <col min="16" max="23" customWidth="true" style="1" width="10.83203125" collapsed="true"/>
+    <col min="24" max="16384" customWidth="true" style="1" width="10.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -1787,6 +1799,9 @@
       <c r="O25" t="n">
         <v>710</v>
       </c>
+      <c r="P25" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:16">
       <c r="A26" t="s">
@@ -2234,19 +2249,22 @@
       <c r="O34" t="n">
         <v>46.6</v>
       </c>
-    </row>
-    <row r="35">
+      <c r="P34" t="n">
+        <v>624.2505119047621</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" t="s">
         <v>53</v>
       </c>
       <c r="B35" t="n">
-        <v>20.649999618530273</v>
+        <v>20.64999961853027</v>
       </c>
       <c r="C35" t="n">
-        <v>82.0</v>
+        <v>82</v>
       </c>
       <c r="D35" t="n">
-        <v>1012.0</v>
+        <v>1012</v>
       </c>
       <c r="E35" t="n">
         <v>4.599999904632568</v>
@@ -2258,28 +2276,178 @@
         <v>31</v>
       </c>
       <c r="H35" t="n">
-        <v>17.299999237060547</v>
+        <v>17.29999923706055</v>
       </c>
       <c r="I35" t="n">
         <v>993.760009765625</v>
       </c>
       <c r="J35" t="n">
-        <v>76.0</v>
+        <v>76</v>
       </c>
       <c r="K35" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" t="n">
+        <v>1.279999971389771</v>
+      </c>
+      <c r="M35" t="n">
+        <v>656.39</v>
+      </c>
+      <c r="N35" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="O35" t="n">
+        <v>46.6</v>
+      </c>
+      <c r="P35" t="n">
+        <v>574.6695773809524</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" t="n">
+        <v>20.3700008392334</v>
+      </c>
+      <c r="C36" t="n">
+        <v>100</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1013</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F36" t="s">
+        <v>31</v>
+      </c>
+      <c r="G36" t="s">
+        <v>55</v>
+      </c>
+      <c r="H36" t="n">
+        <v>12.68000030517578</v>
+      </c>
+      <c r="I36" t="n">
+        <v>994.5700073242188</v>
+      </c>
+      <c r="J36" t="n">
+        <v>92</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" t="n">
+        <v>1.210000038146973</v>
+      </c>
+      <c r="M36" t="n">
+        <v>166.8</v>
+      </c>
+      <c r="N36" t="n">
+        <v>24.1</v>
+      </c>
+      <c r="O36" t="n">
+        <v>459</v>
+      </c>
+      <c r="P36" t="n">
+        <v>695.5120679320678</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" t="n">
+        <v>20.3700008392334</v>
+      </c>
+      <c r="C37" t="n">
+        <v>100</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1013</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F37" t="s">
+        <v>31</v>
+      </c>
+      <c r="G37" t="s">
+        <v>55</v>
+      </c>
+      <c r="H37" t="n">
+        <v>12.68000030517578</v>
+      </c>
+      <c r="I37" t="n">
+        <v>994.5700073242188</v>
+      </c>
+      <c r="J37" t="n">
+        <v>92</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" t="n">
+        <v>1.210000038146973</v>
+      </c>
+      <c r="M37" t="n">
+        <v>166.8</v>
+      </c>
+      <c r="N37" t="n">
+        <v>24</v>
+      </c>
+      <c r="O37" t="n">
+        <v>459</v>
+      </c>
+      <c r="P37" t="n">
+        <v>587.8878928571428</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" t="n">
+        <v>20.3700008392334</v>
+      </c>
+      <c r="C38" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1013.0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F38" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38" t="s">
+        <v>55</v>
+      </c>
+      <c r="H38" t="n">
+        <v>12.680000305175781</v>
+      </c>
+      <c r="I38" t="n">
+        <v>994.5700073242188</v>
+      </c>
+      <c r="J38" t="n">
+        <v>92.0</v>
+      </c>
+      <c r="K38" t="n">
         <v>0.0</v>
       </c>
-      <c r="L35" t="n">
-        <v>1.2799999713897705</v>
-      </c>
-      <c r="M35" t="s">
-        <v>54</v>
-      </c>
-      <c r="N35" t="s">
-        <v>54</v>
-      </c>
-      <c r="O35" t="s">
-        <v>54</v>
+      <c r="L38" t="n">
+        <v>1.2100000381469727</v>
+      </c>
+      <c r="M38" t="s">
+        <v>58</v>
+      </c>
+      <c r="N38" t="s">
+        <v>58</v>
+      </c>
+      <c r="O38" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code for Sending the code from locl system to AWS sytem
</commit_message>
<xml_diff>
--- a/Weather/bin/newFile.xlsx
+++ b/Weather/bin/newFile.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="59" count="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64" count="6">
   <si>
     <t>Time Stamp</t>
   </si>
@@ -63,6 +63,9 @@
     <t>Predicted Value</t>
   </si>
   <si>
+    <t>Running Time</t>
+  </si>
+  <si>
     <t>2017.06.01 20.23.09</t>
   </si>
   <si>
@@ -187,6 +190,18 @@
   </si>
   <si>
     <t>2017.06.03 20.16.06</t>
+  </si>
+  <si>
+    <t>2017.06.07 23.49.04</t>
+  </si>
+  <si>
+    <t>2017-06-08T06:00:00</t>
+  </si>
+  <si>
+    <t>2017-06-08T09:00:00</t>
+  </si>
+  <si>
+    <t>2017.06.08 01.19.29</t>
   </si>
   <si>
     <t/>
@@ -526,10 +541,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView showRuler="0" tabSelected="1" topLeftCell="H16" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView showRuler="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
@@ -549,11 +564,11 @@
     <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="15.1640625" collapsed="true"/>
     <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="24.33203125" collapsed="true"/>
     <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="15.1640625" collapsed="true"/>
-    <col min="16" max="23" customWidth="true" style="1" width="10.83203125" collapsed="true"/>
-    <col min="24" max="16384" customWidth="true" style="1" width="10.83203125" collapsed="true"/>
+    <col min="16" max="24" customWidth="true" style="1" width="10.83203125" collapsed="true"/>
+    <col min="25" max="16384" customWidth="true" style="1" width="10.83203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -602,10 +617,13 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" t="n">
         <v>19.22999954223633</v>
@@ -620,10 +638,10 @@
         <v>2.599999904632568</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" t="n">
         <v>12.6899995803833</v>
@@ -653,9 +671,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" t="n">
         <v>19.22999954223633</v>
@@ -670,10 +688,10 @@
         <v>2.599999904632568</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" t="n">
         <v>12.6899995803833</v>
@@ -703,9 +721,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="n">
         <v>19.22999954223633</v>
@@ -720,10 +738,10 @@
         <v>2.599999904632568</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H4" t="n">
         <v>12.6899995803833</v>
@@ -753,9 +771,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="n">
         <v>19.22999954223633</v>
@@ -770,10 +788,10 @@
         <v>2.599999904632568</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H5" t="n">
         <v>12.6899995803833</v>
@@ -803,9 +821,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" t="n">
         <v>19.22999954223633</v>
@@ -820,10 +838,10 @@
         <v>2.599999904632568</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H6" t="n">
         <v>12.6899995803833</v>
@@ -853,9 +871,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" t="n">
         <v>19.22999954223633</v>
@@ -870,10 +888,10 @@
         <v>2.599999904632568</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H7" t="n">
         <v>12.6899995803833</v>
@@ -903,9 +921,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" t="n">
         <v>19.22999954223633</v>
@@ -920,10 +938,10 @@
         <v>2.599999904632568</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H8" t="n">
         <v>12.6899995803833</v>
@@ -953,9 +971,9 @@
         <v>800</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" t="n">
         <v>19.22999954223633</v>
@@ -970,10 +988,10 @@
         <v>2.599999904632568</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H9" t="n">
         <v>12.6899995803833</v>
@@ -1003,9 +1021,9 @@
         <v>890</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" t="n">
         <v>19.22999954223633</v>
@@ -1020,10 +1038,10 @@
         <v>2.599999904632568</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H10" t="n">
         <v>12.6899995803833</v>
@@ -1053,9 +1071,9 @@
         <v>800</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" t="n">
         <v>19.22999954223633</v>
@@ -1070,10 +1088,10 @@
         <v>2.599999904632568</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H11" t="n">
         <v>12.6899995803833</v>
@@ -1103,9 +1121,9 @@
         <v>847.4545454545456</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" t="n">
         <v>19.22999954223633</v>
@@ -1120,10 +1138,10 @@
         <v>2.599999904632568</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H12" t="n">
         <v>12.6899995803833</v>
@@ -1153,9 +1171,9 @@
         <v>789.279090909091</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" t="n">
         <v>22.6200008392334</v>
@@ -1170,10 +1188,10 @@
         <v>5.699999809265137</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H13" t="n">
         <v>18.59000015258789</v>
@@ -1203,9 +1221,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" t="n">
         <v>22.6200008392334</v>
@@ -1220,10 +1238,10 @@
         <v>5.699999809265137</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H14" t="n">
         <v>18.59000015258789</v>
@@ -1253,9 +1271,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B15" t="n">
         <v>22.6200008392334</v>
@@ -1270,10 +1288,10 @@
         <v>5.699999809265137</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H15" t="n">
         <v>18.59000015258789</v>
@@ -1303,9 +1321,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B16" t="n">
         <v>22.6200008392334</v>
@@ -1320,10 +1338,10 @@
         <v>5.699999809265137</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H16" t="n">
         <v>18.59000015258789</v>
@@ -1353,9 +1371,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B17" t="n">
         <v>22.6200008392334</v>
@@ -1370,10 +1388,10 @@
         <v>5.699999809265137</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H17" t="n">
         <v>18.59000015258789</v>
@@ -1403,9 +1421,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B18" t="n">
         <v>22.6200008392334</v>
@@ -1420,10 +1438,10 @@
         <v>5.699999809265137</v>
       </c>
       <c r="F18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H18" t="n">
         <v>18.59000015258789</v>
@@ -1453,9 +1471,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B19" t="n">
         <v>22.6200008392334</v>
@@ -1470,10 +1488,10 @@
         <v>5.699999809265137</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H19" t="n">
         <v>18.59000015258789</v>
@@ -1503,9 +1521,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B20" t="n">
         <v>22.6200008392334</v>
@@ -1520,10 +1538,10 @@
         <v>5.699999809265137</v>
       </c>
       <c r="F20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H20" t="n">
         <v>18.59000015258789</v>
@@ -1553,9 +1571,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B21" t="n">
         <v>22.6200008392334</v>
@@ -1570,10 +1588,10 @@
         <v>5.699999809265137</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H21" t="n">
         <v>18.59000015258789</v>
@@ -1603,9 +1621,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B22" t="n">
         <v>22.6200008392334</v>
@@ -1620,10 +1638,10 @@
         <v>5.699999809265137</v>
       </c>
       <c r="F22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H22" t="n">
         <v>18.59000015258789</v>
@@ -1653,9 +1671,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B23" t="n">
         <v>22.6200008392334</v>
@@ -1670,10 +1688,10 @@
         <v>5.699999809265137</v>
       </c>
       <c r="F23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H23" t="n">
         <v>18.59000015258789</v>
@@ -1703,9 +1721,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B24" t="n">
         <v>22.6200008392334</v>
@@ -1720,10 +1738,10 @@
         <v>5.699999809265137</v>
       </c>
       <c r="F24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H24" t="n">
         <v>18.59000015258789</v>
@@ -1753,9 +1771,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B25" t="n">
         <v>22.6200008392334</v>
@@ -1770,10 +1788,10 @@
         <v>5.699999809265137</v>
       </c>
       <c r="F25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H25" t="n">
         <v>18.59000015258789</v>
@@ -1803,9 +1821,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B26" t="n">
         <v>22.6200008392334</v>
@@ -1820,10 +1838,10 @@
         <v>5.699999809265137</v>
       </c>
       <c r="F26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H26" t="n">
         <v>18.59000015258789</v>
@@ -1853,9 +1871,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B27" t="n">
         <v>22.6200008392334</v>
@@ -1870,10 +1888,10 @@
         <v>5.699999809265137</v>
       </c>
       <c r="F27" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H27" t="n">
         <v>18.59000015258789</v>
@@ -1903,9 +1921,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B28" t="n">
         <v>21.01000022888184</v>
@@ -1920,10 +1938,10 @@
         <v>4.599999904632568</v>
       </c>
       <c r="F28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H28" t="n">
         <v>17.29999923706055</v>
@@ -1953,9 +1971,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B29" t="n">
         <v>21.01000022888184</v>
@@ -1970,10 +1988,10 @@
         <v>4.599999904632568</v>
       </c>
       <c r="F29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H29" t="n">
         <v>17.29999923706055</v>
@@ -2003,9 +2021,9 @@
         <v>415.7765141700405</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B30" t="n">
         <v>21.01000022888184</v>
@@ -2020,10 +2038,10 @@
         <v>4.599999904632568</v>
       </c>
       <c r="F30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H30" t="n">
         <v>17.29999923706055</v>
@@ -2053,9 +2071,9 @@
         <v>265.9794871794873</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:17">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B31" t="n">
         <v>20.64999961853027</v>
@@ -2070,10 +2088,10 @@
         <v>4.599999904632568</v>
       </c>
       <c r="F31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H31" t="n">
         <v>17.29999923706055</v>
@@ -2103,9 +2121,9 @@
         <v>234</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:17">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B32" t="n">
         <v>20.64999961853027</v>
@@ -2120,10 +2138,10 @@
         <v>4.599999904632568</v>
       </c>
       <c r="F32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H32" t="n">
         <v>17.29999923706055</v>
@@ -2153,9 +2171,9 @@
         <v>624.2505119047621</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:17">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B33" t="n">
         <v>20.64999961853027</v>
@@ -2170,10 +2188,10 @@
         <v>4.599999904632568</v>
       </c>
       <c r="F33" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H33" t="n">
         <v>17.29999923706055</v>
@@ -2203,9 +2221,9 @@
         <v>574.6695773809524</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:17">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B34" t="n">
         <v>20.64999961853027</v>
@@ -2220,10 +2238,10 @@
         <v>4.599999904632568</v>
       </c>
       <c r="F34" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H34" t="n">
         <v>17.29999923706055</v>
@@ -2253,9 +2271,9 @@
         <v>624.2505119047621</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:17">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B35" t="n">
         <v>20.64999961853027</v>
@@ -2270,10 +2288,10 @@
         <v>4.599999904632568</v>
       </c>
       <c r="F35" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H35" t="n">
         <v>17.29999923706055</v>
@@ -2303,9 +2321,9 @@
         <v>574.6695773809524</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:17">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B36" t="n">
         <v>20.3700008392334</v>
@@ -2320,10 +2338,10 @@
         <v>1.5</v>
       </c>
       <c r="F36" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G36" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H36" t="n">
         <v>12.68000030517578</v>
@@ -2353,9 +2371,9 @@
         <v>695.5120679320678</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:17">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B37" t="n">
         <v>20.3700008392334</v>
@@ -2370,10 +2388,10 @@
         <v>1.5</v>
       </c>
       <c r="F37" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G37" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H37" t="n">
         <v>12.68000030517578</v>
@@ -2403,51 +2421,154 @@
         <v>587.8878928571428</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:17">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B38" t="n">
         <v>20.3700008392334</v>
       </c>
       <c r="C38" t="n">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D38" t="n">
-        <v>1013.0</v>
+        <v>1013</v>
       </c>
       <c r="E38" t="n">
         <v>1.5</v>
       </c>
       <c r="F38" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G38" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H38" t="n">
-        <v>12.680000305175781</v>
+        <v>12.68000030517578</v>
       </c>
       <c r="I38" t="n">
         <v>994.5700073242188</v>
       </c>
       <c r="J38" t="n">
-        <v>92.0</v>
+        <v>92</v>
       </c>
       <c r="K38" t="n">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L38" t="n">
-        <v>1.2100000381469727</v>
-      </c>
-      <c r="M38" t="s">
-        <v>58</v>
-      </c>
-      <c r="N38" t="s">
-        <v>58</v>
-      </c>
-      <c r="O38" t="s">
-        <v>58</v>
+        <v>1.210000038146973</v>
+      </c>
+      <c r="M38" t="n">
+        <v>168.9</v>
+      </c>
+      <c r="N38" t="n">
+        <v>22.8</v>
+      </c>
+      <c r="O38" t="n">
+        <v>517</v>
+      </c>
+      <c r="P38" t="n">
+        <v>642.1370561497326</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="A39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" t="n">
+        <v>17</v>
+      </c>
+      <c r="C39" t="n">
+        <v>82</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1015</v>
+      </c>
+      <c r="E39" t="n">
+        <v>3.099999904632568</v>
+      </c>
+      <c r="F39" t="s">
+        <v>60</v>
+      </c>
+      <c r="G39" t="s">
+        <v>61</v>
+      </c>
+      <c r="H39" t="n">
+        <v>14.77000045776367</v>
+      </c>
+      <c r="I39" t="n">
+        <v>997.6500244140625</v>
+      </c>
+      <c r="J39" t="n">
+        <v>94</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.004999999888241291</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0.9200000166893005</v>
+      </c>
+      <c r="M39" t="n">
+        <v>163.7</v>
+      </c>
+      <c r="N39" t="n">
+        <v>24</v>
+      </c>
+      <c r="O39" t="n">
+        <v>458</v>
+      </c>
+      <c r="P39" t="n">
+        <v>782.1946466768526</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>26.51946466768526</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" t="n">
+        <v>16.639999389648438</v>
+      </c>
+      <c r="C40" t="n">
+        <v>82.0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1016.0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F40" t="s">
+        <v>60</v>
+      </c>
+      <c r="G40" t="s">
+        <v>61</v>
+      </c>
+      <c r="H40" t="n">
+        <v>14.479999542236328</v>
+      </c>
+      <c r="I40" t="n">
+        <v>997.6500244140625</v>
+      </c>
+      <c r="J40" t="n">
+        <v>94.0</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0.004999999888241291</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0.9200000166893005</v>
+      </c>
+      <c r="M40" t="s">
+        <v>63</v>
+      </c>
+      <c r="N40" t="s">
+        <v>63</v>
+      </c>
+      <c r="O40" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>